<commit_message>
explanation tweaks in template
</commit_message>
<xml_diff>
--- a/inst/A2SIT_data_input_template.xlsx
+++ b/inst/A2SIT_data_input_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/42dcc5b33b6ca4b2/Work/Guatemala/2_App/A2SIT/inst/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="244" documentId="8_{40DD6BD8-3AB8-4283-834B-8C3A994CC4BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{14B67CC7-052E-4766-A7AA-A3AE6E77E42B}"/>
+  <xr:revisionPtr revIDLastSave="256" documentId="8_{40DD6BD8-3AB8-4283-834B-8C3A994CC4BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0F5F2AE2-22B3-419F-9C92-E424B769DB2C}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -836,7 +836,7 @@
           </a:r>
           <a:r>
             <a:rPr lang="en-GB" sz="1100" b="0" i="0" baseline="0"/>
-            <a:t> of the indicator. Weights are relative within groups, and some reweighting can be done within the app. Unless you have a clear idea of indicator weights, set all of these to 1 for equal indicator weighting.</a:t>
+            <a:t> of the indicator. Weights are relative within groups. Unless you have a clear idea of indicator weights, set all of these to 1 for equal indicator weighting.</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -1006,25 +1006,57 @@
         <a:p>
           <a:r>
             <a:rPr lang="en-GB" sz="1100" baseline="0"/>
-            <a:t>- The iCode column gives the code of the group, which should be unique</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
+            <a:t>- The </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" b="1" baseline="0"/>
+            <a:t>iCode</a:t>
+          </a:r>
           <a:r>
             <a:rPr lang="en-GB" sz="1100" baseline="0"/>
-            <a:t>- The iName column gives the corresponding full name of the iCode</a:t>
+            <a:t> column gives the code of the group, which should be unique</a:t>
           </a:r>
         </a:p>
         <a:p>
           <a:r>
             <a:rPr lang="en-GB" sz="1100" baseline="0"/>
-            <a:t>- The Parent column defines which aggregation group the iCode belongs to, in the level immediately above</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
+            <a:t>- The </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" b="1" baseline="0"/>
+            <a:t>iName</a:t>
+          </a:r>
           <a:r>
             <a:rPr lang="en-GB" sz="1100" baseline="0"/>
-            <a:t>- The Level column defines the level of the index for the iCode, where 1 is the indicator level, 2 is the level immediately above indicators, and so on.</a:t>
+            <a:t> column gives the corresponding full name of the iCode</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" baseline="0"/>
+            <a:t>- The </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" b="1" baseline="0"/>
+            <a:t>Parent</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" baseline="0"/>
+            <a:t> column defines which aggregation group the iCode belongs to, in the level immediately above. Each indicator/group should have a parent which is not at the same level or below. For example, an indicator in level 1 should have a parent at level 2. An aggregation group at level 2 should have a parent at level 3, and so on.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" baseline="0"/>
+            <a:t>- The </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" b="1" baseline="0"/>
+            <a:t>Level</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" baseline="0"/>
+            <a:t> column defines the level of the index for the iCode, where 1 is the indicator level, 2 is the level immediately above indicators, and so on.</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -1112,16 +1144,13 @@
         <a:p>
           <a:r>
             <a:rPr lang="en-GB" sz="1100" baseline="0"/>
-            <a:t>   - The User Guide </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-GB" sz="1100" baseline="0">
-              <a:solidFill>
-                <a:srgbClr val="FF0000"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t>[TO ADD]</a:t>
-          </a:r>
+            <a:t>   - The User Guide: https://unhcr-guatemala.github.io/A2SIT/book/index.html</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-GB" sz="1100" baseline="0">
+            <a:solidFill>
+              <a:srgbClr val="FF0000"/>
+            </a:solidFill>
+          </a:endParaRPr>
         </a:p>
         <a:p>
           <a:r>
@@ -1174,10 +1203,6 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3210,15 +3235,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100748193D12EBC014087ABC46D0B7ADDF5" ma:contentTypeVersion="16" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="124c5de7df4a247e685b680f9ee11a62">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="4c567442-fa22-4cbd-8da7-89fd320ef710" xmlns:ns3="29371e11-ecd1-431d-9bd3-d4d03d3b040e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="ca14ef562ffe71505030771d2853299b" ns2:_="" ns3:_="">
     <xsd:import namespace="4c567442-fa22-4cbd-8da7-89fd320ef710"/>
@@ -3461,15 +3477,16 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0955C5F8-E177-4943-AFA7-4E170F303478}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{08F6FAC0-2D0A-4DC9-9BEE-D7FFD540AA8B}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3486,4 +3503,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0955C5F8-E177-4943-AFA7-4E170F303478}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>